<commit_message>
Adding to the GUI
</commit_message>
<xml_diff>
--- a/Synthetic Data.xlsx
+++ b/Synthetic Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joaod\Documents\GitHub\synthetic-goalkeeping-data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E01B813C-60FF-4A5C-A628-C75DF90DD5D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12CC9EC7-C0D8-4819-BBCE-DB6E9D725750}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{F525CFEA-FD6C-42D5-8121-36B5EA7DB628}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="20">
   <si>
     <t>Neutro</t>
   </si>
@@ -94,9 +94,6 @@
   </si>
   <si>
     <t>y</t>
-  </si>
-  <si>
-    <t>isgoal</t>
   </si>
   <si>
     <t>appearance</t>
@@ -143,10 +140,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -636,15 +632,18 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F834B986-7991-4981-AC5F-29AF8FB25D13}">
-  <dimension ref="A1:G10"/>
+  <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+      <selection activeCell="D1" sqref="D1:D1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="4" max="4" width="8.7265625" style="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>16</v>
       </c>
@@ -654,14 +653,11 @@
       <c r="C1" t="s">
         <v>18</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="E1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -671,14 +667,11 @@
       <c r="C2">
         <v>7</v>
       </c>
-      <c r="D2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="D2" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -688,15 +681,12 @@
       <c r="C3">
         <v>25</v>
       </c>
-      <c r="D3" t="b">
-        <v>1</v>
-      </c>
-      <c r="E3">
-        <v>0</v>
-      </c>
-      <c r="G3" s="1"/>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="D3" s="1">
+        <v>0</v>
+      </c>
+      <c r="F3" s="1"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -706,15 +696,11 @@
       <c r="C4">
         <v>7</v>
       </c>
-      <c r="D4" t="b">
-        <v>1</v>
-      </c>
-      <c r="E4">
-        <v>0</v>
-      </c>
-      <c r="G4" s="2"/>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="D4" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -724,14 +710,11 @@
       <c r="C5">
         <v>7</v>
       </c>
-      <c r="D5" t="b">
-        <v>1</v>
-      </c>
-      <c r="E5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="D5" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -741,14 +724,11 @@
       <c r="C6">
         <v>1</v>
       </c>
-      <c r="D6" t="b">
-        <v>0</v>
-      </c>
-      <c r="E6">
+      <c r="D6" s="1">
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>8</v>
       </c>
@@ -758,14 +738,11 @@
       <c r="C7">
         <v>20</v>
       </c>
-      <c r="D7" t="b">
-        <v>0</v>
-      </c>
-      <c r="E7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="D7" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>9</v>
       </c>
@@ -775,14 +752,11 @@
       <c r="C8">
         <v>20</v>
       </c>
-      <c r="D8" t="b">
-        <v>0</v>
-      </c>
-      <c r="E8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="D8" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>10</v>
       </c>
@@ -792,14 +766,11 @@
       <c r="C9">
         <v>16</v>
       </c>
-      <c r="D9" t="b">
-        <v>0</v>
-      </c>
-      <c r="E9">
+      <c r="D9" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>11</v>
       </c>
@@ -809,10 +780,7 @@
       <c r="C10">
         <v>5</v>
       </c>
-      <c r="D10" t="b">
-        <v>1</v>
-      </c>
-      <c r="E10">
+      <c r="D10" s="1">
         <v>0</v>
       </c>
     </row>

</xml_diff>